<commit_message>
MA0501: Ajuste de errores de Esqueleto de guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado05/guion01/EsqueletoGuion_MA_05_01_CO.xlsx
+++ b/fuentes/contenidos/grado05/guion01/EsqueletoGuion_MA_05_01_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\Matematicas\fuentes\contenidos\grado05\guion01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\psf\Home\Documents\Aula Planeta Colombia\Repositorios\Matematicas\fuentes\contenidos\grado05\guion01\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7635" tabRatio="729"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19203" windowHeight="7637" tabRatio="729"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="CUADERNO DEL PROFESOR" sheetId="15" r:id="rId4"/>
     <sheet name="CUADERNO DE ESTUDIO" sheetId="16" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="83">
   <si>
     <t>FICHA</t>
   </si>
@@ -246,9 +246,6 @@
     <t>Competencias: aplicación de tipos de conjuntos y operaciones y relaciones entre conjuntos</t>
   </si>
   <si>
-    <t>Mapa conceptual del tema Conjuntos</t>
-  </si>
-  <si>
     <t>Determinación de un conjunto por comprensión</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
   </si>
   <si>
     <t>Conjunto universal o referencial</t>
-  </si>
-  <si>
-    <t>Relaciones entre conjuntos. Conjuntos disjuntos y conjuntos intersecantes</t>
   </si>
   <si>
     <t>Conjuntos disjuntos</t>
@@ -842,7 +836,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -925,6 +919,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="401">
@@ -1609,16 +1606,16 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" customWidth="1"/>
-    <col min="2" max="2" width="104.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.3984375" customWidth="1"/>
+    <col min="2" max="2" width="104.265625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="12" t="s">
         <v>8</v>
       </c>
@@ -1626,7 +1623,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A2" s="12" t="s">
         <v>9</v>
       </c>
@@ -1634,7 +1631,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="12" t="s">
         <v>10</v>
       </c>
@@ -1642,7 +1639,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A4" s="12" t="s">
         <v>11</v>
       </c>
@@ -1650,7 +1647,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1658,7 +1655,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A6" s="12" t="s">
         <v>12</v>
       </c>
@@ -1685,19 +1682,19 @@
       <selection activeCell="C12" sqref="C12:C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="64.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20.42578125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="64.73046875" customWidth="1"/>
+    <col min="5" max="5" width="20.3984375" customWidth="1"/>
+    <col min="7" max="7" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="15.1328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.73046875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>1</v>
       </c>
@@ -1717,7 +1714,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="13"/>
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
@@ -1731,7 +1728,7 @@
       <c r="K2"/>
       <c r="L2"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" s="13"/>
       <c r="B3" s="13"/>
       <c r="C3" s="13"/>
@@ -1739,7 +1736,7 @@
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" s="14"/>
       <c r="B4" s="14"/>
       <c r="C4" s="14"/>
@@ -1747,7 +1744,7 @@
       <c r="E4" s="14"/>
       <c r="F4" s="14"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="C5" s="15"/>
@@ -1755,16 +1752,16 @@
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G9" s="7"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G10" s="7"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G11" s="7"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="G12" s="7"/>
     </row>
   </sheetData>
@@ -1783,16 +1780,16 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C2" sqref="C2:C26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="66.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="66.1328125" customWidth="1"/>
+    <col min="2" max="2" width="14.73046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="11" t="s">
         <v>3</v>
       </c>
@@ -1803,278 +1800,278 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" s="5">
+      <c r="B2" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="37">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="5">
+      <c r="B3" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="37">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="37">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="37">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="37">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="5">
+      <c r="B7" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="37">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C8" s="5">
+      <c r="B8" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="37">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="37">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="37">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5">
+      <c r="B11" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="37">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="5">
+      <c r="B12" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12" s="37">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="5">
+      <c r="B13" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="37">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B14" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="5">
+      <c r="B14" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="37">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="5">
+      <c r="B15" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="37">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" s="5">
+      <c r="B16" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="37">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="37">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="5">
+      <c r="B18" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C18" s="37">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="37" t="s">
         <v>61</v>
       </c>
-      <c r="C19" s="5">
+      <c r="C19" s="37">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C20" s="5">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20" s="37">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="37">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="5">
+      <c r="B22" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="37">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B23" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="5">
+      <c r="B23" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="37">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="B24" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C24" s="5">
+      <c r="B24" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C24" s="37">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="5">
+        <v>20</v>
+      </c>
+      <c r="B25" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="37">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="5">
+      <c r="B26" s="37" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="37">
         <v>25</v>
       </c>
     </row>
@@ -2099,18 +2096,18 @@
   </sheetPr>
   <dimension ref="A1:C31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="92.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="6" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.265625" customWidth="1"/>
+    <col min="3" max="3" width="19.265625" style="6" customWidth="1"/>
+    <col min="4" max="4" width="23.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>5</v>
       </c>
@@ -2121,7 +2118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -2132,7 +2129,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -2143,7 +2140,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -2154,7 +2151,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -2165,7 +2162,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -2176,7 +2173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -2187,7 +2184,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -2198,7 +2195,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -2209,7 +2206,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -2220,7 +2217,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -2231,7 +2228,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -2242,7 +2239,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -2253,7 +2250,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" s="5">
         <v>13</v>
       </c>
@@ -2264,7 +2261,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" s="5">
         <v>14</v>
       </c>
@@ -2275,7 +2272,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" s="5">
         <v>15</v>
       </c>
@@ -2286,7 +2283,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A17" s="5">
         <v>16</v>
       </c>
@@ -2297,7 +2294,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A18" s="26">
         <v>17</v>
       </c>
@@ -2308,7 +2305,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A19" s="5">
         <v>18</v>
       </c>
@@ -2319,7 +2316,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A20" s="5">
         <v>19</v>
       </c>
@@ -2330,7 +2327,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A21" s="5">
         <v>20</v>
       </c>
@@ -2341,7 +2338,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A22" s="5">
         <v>21</v>
       </c>
@@ -2352,7 +2349,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A23" s="5">
         <v>22</v>
       </c>
@@ -2363,7 +2360,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A24" s="5">
         <v>23</v>
       </c>
@@ -2374,18 +2371,18 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A25" s="5">
         <v>24</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A26" s="5">
         <v>25</v>
       </c>
@@ -2396,23 +2393,23 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A27" s="25"/>
       <c r="B27" s="25"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A28" s="25"/>
       <c r="B28" s="25"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A29" s="25"/>
       <c r="B29" s="25"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A30" s="25"/>
       <c r="B30" s="25"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A31" s="25"/>
       <c r="B31" s="25"/>
     </row>
@@ -2435,24 +2432,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46:A53"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" customWidth="1"/>
-    <col min="2" max="2" width="51.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="45.5703125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="36.28515625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="64.140625" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.86328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="28.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="45.59765625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="17.86328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="36.265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="17.86328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="64.1328125" customWidth="1"/>
+    <col min="9" max="9" width="17.3984375" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.85" x14ac:dyDescent="0.5">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
@@ -2481,7 +2478,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="16" t="s">
         <v>28</v>
       </c>
@@ -2498,7 +2495,7 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
     </row>
-    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="16" t="s">
         <v>28</v>
       </c>
@@ -2515,7 +2512,7 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
     </row>
-    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A4" s="16" t="s">
         <v>28</v>
       </c>
@@ -2532,7 +2529,7 @@
       <c r="H4" s="19"/>
       <c r="I4" s="13"/>
     </row>
-    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A5" s="16" t="s">
         <v>28</v>
       </c>
@@ -2553,7 +2550,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A6" s="16" t="s">
         <v>28</v>
       </c>
@@ -2570,7 +2567,7 @@
       <c r="H6" s="19"/>
       <c r="I6" s="13"/>
     </row>
-    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7" s="16" t="s">
         <v>28</v>
       </c>
@@ -2587,7 +2584,7 @@
       <c r="H7" s="19"/>
       <c r="I7" s="17"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="16" t="s">
         <v>28</v>
       </c>
@@ -2608,7 +2605,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A9" s="16" t="s">
         <v>28</v>
       </c>
@@ -2627,7 +2624,7 @@
       <c r="H9" s="19"/>
       <c r="I9" s="13"/>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="16" t="s">
         <v>28</v>
       </c>
@@ -2648,7 +2645,7 @@
       <c r="H10" s="19"/>
       <c r="I10" s="13"/>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="16" t="s">
         <v>28</v>
       </c>
@@ -2673,7 +2670,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="16" t="s">
         <v>28</v>
       </c>
@@ -2686,7 +2683,7 @@
       </c>
       <c r="E12" s="19"/>
       <c r="F12" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G12" s="19" t="s">
         <v>22</v>
@@ -2694,7 +2691,7 @@
       <c r="H12" s="19"/>
       <c r="I12" s="13"/>
     </row>
-    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A13" s="16" t="s">
         <v>28</v>
       </c>
@@ -2707,7 +2704,7 @@
       </c>
       <c r="E13" s="19"/>
       <c r="F13" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G13" s="19" t="s">
         <v>23</v>
@@ -2715,7 +2712,7 @@
       <c r="H13" s="19"/>
       <c r="I13" s="13"/>
     </row>
-    <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14" s="16" t="s">
         <v>28</v>
       </c>
@@ -2728,7 +2725,7 @@
       </c>
       <c r="E14" s="19"/>
       <c r="F14" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>27</v>
@@ -2736,7 +2733,7 @@
       <c r="H14" s="19"/>
       <c r="I14" s="13"/>
     </row>
-    <row r="15" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="16" t="s">
         <v>28</v>
       </c>
@@ -2749,7 +2746,7 @@
       </c>
       <c r="E15" s="19"/>
       <c r="F15" s="35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G15" s="19" t="s">
         <v>24</v>
@@ -2761,7 +2758,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="16" t="s">
         <v>28</v>
       </c>
@@ -2780,7 +2777,7 @@
       <c r="H16" s="19"/>
       <c r="I16" s="13"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="16" t="s">
         <v>28</v>
       </c>
@@ -2799,7 +2796,7 @@
       <c r="H17" s="17"/>
       <c r="I17" s="16"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="16" t="s">
         <v>28</v>
       </c>
@@ -2818,7 +2815,7 @@
       <c r="H18" s="19"/>
       <c r="I18" s="16"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="16" t="s">
         <v>28</v>
       </c>
@@ -2841,7 +2838,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20" s="16" t="s">
         <v>28</v>
       </c>
@@ -2864,7 +2861,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="28" t="s">
         <v>28</v>
       </c>
@@ -2881,7 +2878,7 @@
       <c r="H21" s="33"/>
       <c r="I21" s="28"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="28" t="s">
         <v>28</v>
       </c>
@@ -2890,7 +2887,7 @@
       </c>
       <c r="C22" s="28"/>
       <c r="D22" s="28" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>22</v>
@@ -2900,7 +2897,7 @@
       <c r="H22" s="28"/>
       <c r="I22" s="28"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="28" t="s">
         <v>28</v>
       </c>
@@ -2909,7 +2906,7 @@
       </c>
       <c r="C23" s="28"/>
       <c r="D23" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>22</v>
@@ -2919,12 +2916,16 @@
       <c r="H23" s="28"/>
       <c r="I23" s="28"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="28"/>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>51</v>
+      </c>
       <c r="C24" s="28"/>
       <c r="D24" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>23</v>
@@ -2934,7 +2935,7 @@
       <c r="H24" s="28"/>
       <c r="I24" s="28"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="28" t="s">
         <v>28</v>
       </c>
@@ -2943,7 +2944,7 @@
       </c>
       <c r="C25" s="28"/>
       <c r="D25" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E25" s="28" t="s">
         <v>22</v>
@@ -2953,7 +2954,7 @@
       <c r="H25" s="28"/>
       <c r="I25" s="28"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="28" t="s">
         <v>28</v>
       </c>
@@ -2962,7 +2963,7 @@
       </c>
       <c r="C26" s="28"/>
       <c r="D26" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E26" s="28" t="s">
         <v>23</v>
@@ -2972,7 +2973,7 @@
       <c r="H26" s="28"/>
       <c r="I26" s="28"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="28" t="s">
         <v>28</v>
       </c>
@@ -2981,7 +2982,7 @@
       </c>
       <c r="C27" s="28"/>
       <c r="D27" s="28" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E27" s="28" t="s">
         <v>26</v>
@@ -2995,7 +2996,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="28" t="s">
         <v>28</v>
       </c>
@@ -3004,7 +3005,7 @@
       </c>
       <c r="C28" s="28"/>
       <c r="D28" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E28" s="28" t="s">
         <v>22</v>
@@ -3014,7 +3015,7 @@
       <c r="H28" s="28"/>
       <c r="I28" s="28"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="28" t="s">
         <v>28</v>
       </c>
@@ -3023,7 +3024,7 @@
       </c>
       <c r="C29" s="28"/>
       <c r="D29" s="28" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E29" s="28" t="s">
         <v>23</v>
@@ -3033,7 +3034,7 @@
       <c r="H29" s="28"/>
       <c r="I29" s="28"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="28" t="s">
         <v>28</v>
       </c>
@@ -3042,7 +3043,7 @@
       </c>
       <c r="C30" s="28"/>
       <c r="D30" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E30" s="28" t="s">
         <v>22</v>
@@ -3052,7 +3053,7 @@
       <c r="H30" s="28"/>
       <c r="I30" s="28"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="28" t="s">
         <v>28</v>
       </c>
@@ -3061,7 +3062,7 @@
       </c>
       <c r="C31" s="28"/>
       <c r="D31" s="28" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E31" s="28" t="s">
         <v>23</v>
@@ -3071,7 +3072,7 @@
       <c r="H31" s="28"/>
       <c r="I31" s="28"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="28" t="s">
         <v>28</v>
       </c>
@@ -3080,7 +3081,7 @@
       </c>
       <c r="C32" s="28"/>
       <c r="D32" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>22</v>
@@ -3090,7 +3091,7 @@
       <c r="H32" s="28"/>
       <c r="I32" s="28"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="28" t="s">
         <v>28</v>
       </c>
@@ -3099,7 +3100,7 @@
       </c>
       <c r="C33" s="28"/>
       <c r="D33" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E33" s="28" t="s">
         <v>23</v>
@@ -3109,7 +3110,7 @@
       <c r="H33" s="28"/>
       <c r="I33" s="28"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="28" t="s">
         <v>28</v>
       </c>
@@ -3128,7 +3129,7 @@
       <c r="H34" s="28"/>
       <c r="I34" s="28"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="28" t="s">
         <v>28</v>
       </c>
@@ -3151,7 +3152,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="28" t="s">
         <v>28</v>
       </c>
@@ -3174,7 +3175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="20" t="s">
         <v>28</v>
       </c>
@@ -3191,7 +3192,7 @@
       <c r="H37" s="20"/>
       <c r="I37" s="20"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="20" t="s">
         <v>28</v>
       </c>
@@ -3210,7 +3211,7 @@
       <c r="H38" s="20"/>
       <c r="I38" s="20"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="20" t="s">
         <v>28</v>
       </c>
@@ -3229,7 +3230,7 @@
       <c r="H39" s="20"/>
       <c r="I39" s="20"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="20" t="s">
         <v>28</v>
       </c>
@@ -3248,7 +3249,7 @@
       <c r="H40" s="20"/>
       <c r="I40" s="20"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="20" t="s">
         <v>28</v>
       </c>
@@ -3267,7 +3268,7 @@
       <c r="H41" s="20"/>
       <c r="I41" s="20"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="20" t="s">
         <v>28</v>
       </c>
@@ -3290,7 +3291,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="20" t="s">
         <v>28</v>
       </c>
@@ -3313,7 +3314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="20" t="s">
         <v>28</v>
       </c>
@@ -3332,7 +3333,7 @@
       <c r="H44" s="20"/>
       <c r="I44" s="20"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="20" t="s">
         <v>28</v>
       </c>
@@ -3351,7 +3352,7 @@
       <c r="H45" s="20"/>
       <c r="I45" s="20"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="20" t="s">
         <v>28</v>
       </c>
@@ -3374,7 +3375,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="20" t="s">
         <v>28</v>
       </c>
@@ -3383,7 +3384,7 @@
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E47" s="20" t="s">
         <v>22</v>
@@ -3393,7 +3394,7 @@
       <c r="H47" s="20"/>
       <c r="I47" s="20"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="20" t="s">
         <v>28</v>
       </c>
@@ -3402,7 +3403,7 @@
       </c>
       <c r="C48" s="20"/>
       <c r="D48" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E48" s="20" t="s">
         <v>25</v>
@@ -3412,7 +3413,7 @@
       <c r="H48" s="20"/>
       <c r="I48" s="20"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="20" t="s">
         <v>28</v>
       </c>
@@ -3421,7 +3422,7 @@
       </c>
       <c r="C49" s="20"/>
       <c r="D49" s="20" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E49" s="20" t="s">
         <v>23</v>
@@ -3431,7 +3432,7 @@
       <c r="H49" s="20"/>
       <c r="I49" s="20"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="20" t="s">
         <v>28</v>
       </c>
@@ -3440,7 +3441,7 @@
       </c>
       <c r="C50" s="20"/>
       <c r="D50" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E50" s="20" t="s">
         <v>22</v>
@@ -3450,7 +3451,7 @@
       <c r="H50" s="20"/>
       <c r="I50" s="20"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="20" t="s">
         <v>28</v>
       </c>
@@ -3459,7 +3460,7 @@
       </c>
       <c r="C51" s="20"/>
       <c r="D51" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E51" s="20" t="s">
         <v>25</v>
@@ -3469,7 +3470,7 @@
       <c r="H51" s="20"/>
       <c r="I51" s="20"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="20" t="s">
         <v>28</v>
       </c>
@@ -3478,7 +3479,7 @@
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E52" s="20" t="s">
         <v>23</v>
@@ -3488,7 +3489,7 @@
       <c r="H52" s="20"/>
       <c r="I52" s="20"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="20" t="s">
         <v>28</v>
       </c>
@@ -3497,7 +3498,7 @@
       </c>
       <c r="C53" s="20"/>
       <c r="D53" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E53" s="20" t="s">
         <v>26</v>
@@ -3511,7 +3512,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="20" t="s">
         <v>28</v>
       </c>
@@ -3520,7 +3521,7 @@
       </c>
       <c r="C54" s="20"/>
       <c r="D54" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E54" s="20" t="s">
         <v>26</v>
@@ -3534,7 +3535,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="20" t="s">
         <v>28</v>
       </c>
@@ -3543,7 +3544,7 @@
       </c>
       <c r="C55" s="20"/>
       <c r="D55" s="20" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E55" s="20" t="s">
         <v>26</v>
@@ -3557,7 +3558,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="20" t="s">
         <v>28</v>
       </c>
@@ -3576,7 +3577,7 @@
       <c r="H56" s="20"/>
       <c r="I56" s="23"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="20" t="s">
         <v>28</v>
       </c>
@@ -3599,7 +3600,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="20" t="s">
         <v>28</v>
       </c>
@@ -3622,12 +3623,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B59" s="29" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="C59" s="24" t="s">
         <v>22</v>
@@ -3639,7 +3640,7 @@
       <c r="H59" s="24"/>
       <c r="I59" s="24"/>
     </row>
-    <row r="60" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="28" t="s">
         <v>28</v>
       </c>
@@ -3656,7 +3657,7 @@
       <c r="H60" s="24"/>
       <c r="I60" s="24"/>
     </row>
-    <row r="61" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="28" t="s">
         <v>28</v>
       </c>
@@ -3675,7 +3676,7 @@
       <c r="H61" s="24"/>
       <c r="I61" s="24"/>
     </row>
-    <row r="62" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="28" t="s">
         <v>28</v>
       </c>
@@ -3694,7 +3695,7 @@
       <c r="H62" s="24"/>
       <c r="I62" s="24"/>
     </row>
-    <row r="63" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="28" t="s">
         <v>28</v>
       </c>
@@ -3713,7 +3714,7 @@
       <c r="H63" s="30"/>
       <c r="I63" s="24"/>
     </row>
-    <row r="64" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="28" t="s">
         <v>28</v>
       </c>
@@ -3736,7 +3737,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="28" t="s">
         <v>28</v>
       </c>
@@ -3755,7 +3756,7 @@
       <c r="H65" s="30"/>
       <c r="I65" s="24"/>
     </row>
-    <row r="66" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="28" t="s">
         <v>28</v>
       </c>
@@ -3774,7 +3775,7 @@
       <c r="H66" s="24"/>
       <c r="I66" s="24"/>
     </row>
-    <row r="67" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="28" t="s">
         <v>28</v>
       </c>
@@ -3793,7 +3794,7 @@
       <c r="H67" s="24"/>
       <c r="I67" s="24"/>
     </row>
-    <row r="68" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="28" t="s">
         <v>28</v>
       </c>
@@ -3806,7 +3807,7 @@
       </c>
       <c r="E68" s="24"/>
       <c r="F68" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G68" s="24" t="s">
         <v>22</v>
@@ -3814,7 +3815,7 @@
       <c r="H68" s="24"/>
       <c r="I68" s="24"/>
     </row>
-    <row r="69" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="28" t="s">
         <v>28</v>
       </c>
@@ -3827,7 +3828,7 @@
       </c>
       <c r="E69" s="24"/>
       <c r="F69" s="24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G69" s="24" t="s">
         <v>22</v>
@@ -3835,7 +3836,7 @@
       <c r="H69" s="24"/>
       <c r="I69" s="24"/>
     </row>
-    <row r="70" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="28" t="s">
         <v>28</v>
       </c>
@@ -3858,7 +3859,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="71" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="28" t="s">
         <v>28</v>
       </c>
@@ -3877,7 +3878,7 @@
       <c r="H71" s="24"/>
       <c r="I71" s="24"/>
     </row>
-    <row r="72" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="28" t="s">
         <v>28</v>
       </c>
@@ -3900,12 +3901,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B73" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C73" s="24" t="s">
         <v>22</v>
@@ -3917,12 +3918,12 @@
       <c r="H73" s="24"/>
       <c r="I73" s="24"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B74" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C74" s="24" t="s">
         <v>26</v>
@@ -3938,12 +3939,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B75" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C75" s="31" t="s">
         <v>26</v>
@@ -3959,12 +3960,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="28" t="s">
         <v>28</v>
       </c>
       <c r="B76" s="30" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C76" s="24" t="s">
         <v>26</v>
@@ -3980,12 +3981,12 @@
         <v>19</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B77" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>20</v>
@@ -3994,19 +3995,17 @@
       <c r="E77" s="14"/>
       <c r="F77" s="14"/>
       <c r="G77" s="14"/>
-      <c r="H77" s="14" t="s">
-        <v>71</v>
-      </c>
+      <c r="H77" s="14"/>
       <c r="I77" s="14" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="27" t="s">
         <v>28</v>
       </c>
       <c r="B78" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>21</v>

</xml_diff>